<commit_message>
final push of data up
</commit_message>
<xml_diff>
--- a/Fruit_Go_Bad_Dates.xlsx
+++ b/Fruit_Go_Bad_Dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\houst\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\houst\Documents\Github\Computer_Architecture_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E48E0BB-5D61-461B-9BB0-7A3EE41C8D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB91D8C6-124B-4446-BF75-7F4DD7381073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2E06A38C-336B-4ABA-949C-41B707201D5D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{2E06A38C-336B-4ABA-949C-41B707201D5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
   <si>
     <t>Fruit</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>https://kickassbaker.com/how-long-does-watermelon-last-in-the-fridge/</t>
+  </si>
+  <si>
+    <t>https://www.allrecipes.com/article/how-to-store-eggplant/</t>
   </si>
 </sst>
 </file>
@@ -687,19 +690,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBB0C16-F86D-452E-A0AC-ED648EB3DFBA}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +731,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -754,7 +757,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -773,11 +776,11 @@
       <c r="F3">
         <v>84</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -800,7 +803,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -826,7 +829,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -852,7 +855,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -878,7 +881,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -901,7 +904,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -924,7 +927,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -947,7 +950,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -972,11 +975,11 @@
       <c r="H11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -998,11 +1001,11 @@
       <c r="H12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1024,8 +1027,11 @@
       <c r="H13" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1169,7 +1175,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1192,7 +1198,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1238,7 +1244,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1261,7 +1267,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1304,7 +1310,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1327,7 +1333,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1353,7 +1359,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1376,7 +1382,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1399,7 +1405,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1422,7 +1428,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1445,7 +1451,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1468,7 +1474,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1491,7 +1497,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1514,7 +1520,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1540,7 +1546,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1563,7 +1569,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1632,7 +1638,11 @@
     <hyperlink ref="H36" r:id="rId39" xr:uid="{5CBF238A-3F56-400C-A801-DB92BC43DEE3}"/>
     <hyperlink ref="I37" r:id="rId40" xr:uid="{F17C575C-8F30-4ECF-8E0B-DB7A7826B718}"/>
     <hyperlink ref="H37" r:id="rId41" xr:uid="{ACB54725-503C-4383-9A2A-EA2BBD876C1D}"/>
+    <hyperlink ref="H3" r:id="rId42" xr:uid="{472E99B6-5145-4646-A6BF-725565BAA763}"/>
+    <hyperlink ref="I11" r:id="rId43" xr:uid="{B6B18BE6-2D42-40FF-9A81-07AED4FF2547}"/>
+    <hyperlink ref="I12" r:id="rId44" xr:uid="{225CE89C-8E3A-4858-9655-46797B7F97E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>